<commit_message>
added sequence raw QC file
</commit_message>
<xml_diff>
--- a/data/rna_seq/NCBI_upload/Hawaii2023_SRA_metadata.xlsx
+++ b/data/rna_seq/NCBI_upload/Hawaii2023_SRA_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/larval_symbiont_TPC/data/rna_seq/NCBI_upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EA2FF7-59F6-844C-A14D-1302CE58B139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD227AD4-7363-9C41-9CED-EE94F1C14B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8780" yWindow="840" windowWidth="20720" windowHeight="17540" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33500" yWindow="-1440" windowWidth="29560" windowHeight="17540" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact Info and Instructions" sheetId="3" r:id="rId1"/>
@@ -1698,12 +1698,6 @@
     <t>R73_R2_001.fastq.gz</t>
   </si>
   <si>
-    <t>R74_R1_001.fastq.gZ</t>
-  </si>
-  <si>
-    <t>R74_R2_001.fastq.gZ</t>
-  </si>
-  <si>
     <t>R75_R1_001.fastq.gz</t>
   </si>
   <si>
@@ -1722,12 +1716,6 @@
     <t>R77_R2_001.fastq.gz</t>
   </si>
   <si>
-    <t>R78_R1_001.fastq.gZ</t>
-  </si>
-  <si>
-    <t>R78_R2_001.fastq.gZ</t>
-  </si>
-  <si>
     <t>R79_R1_001.fastq.gz</t>
   </si>
   <si>
@@ -1906,6 +1894,18 @@
   </si>
   <si>
     <t>R108_R2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>R74_R2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>R78_R2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>R74_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>R78_R1_001.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -2367,6 +2367,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="62"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="62" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2391,7 +2392,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="77">
     <cellStyle name="40% - Accent1" xfId="3" builtinId="31"/>
@@ -2924,52 +2924,52 @@
       </c>
     </row>
     <row r="3" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="39" t="s">
         <v>197</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
     </row>
     <row r="4" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="39" t="s">
         <v>198</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="40" t="s">
         <v>199</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
     </row>
     <row r="6" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
     </row>
     <row r="7" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="21" t="s">
@@ -3029,15 +3029,15 @@
       </c>
     </row>
     <row r="17" spans="2:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
     </row>
     <row r="18" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="19" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3069,27 +3069,27 @@
       <c r="B37" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="C37" s="36" t="s">
+      <c r="C37" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="D37" s="37"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="37"/>
-      <c r="H37" s="37"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="C38" s="36" t="s">
+      <c r="C38" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="D38" s="37"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="37"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
     </row>
     <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" s="21" t="s">
@@ -3161,8 +3161,8 @@
   <dimension ref="A1:Q286"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L11" sqref="L11"/>
+      <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3244,7 +3244,7 @@
       <c r="B2" t="s">
         <v>294</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="36" t="s">
         <v>295</v>
       </c>
       <c r="D2" s="11" t="s">
@@ -3263,7 +3263,7 @@
         <v>6</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J2" s="12" t="s">
         <v>403</v>
@@ -3285,7 +3285,7 @@
       <c r="B3" t="s">
         <v>296</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="36" t="s">
         <v>297</v>
       </c>
       <c r="D3" s="11" t="s">
@@ -3304,7 +3304,7 @@
         <v>6</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J3" s="12" t="s">
         <v>403</v>
@@ -3326,7 +3326,7 @@
       <c r="B4" t="s">
         <v>298</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="36" t="s">
         <v>299</v>
       </c>
       <c r="D4" s="11" t="s">
@@ -3345,7 +3345,7 @@
         <v>6</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J4" s="12" t="s">
         <v>403</v>
@@ -3367,7 +3367,7 @@
       <c r="B5" t="s">
         <v>300</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="36" t="s">
         <v>301</v>
       </c>
       <c r="D5" s="11" t="s">
@@ -3386,7 +3386,7 @@
         <v>6</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J5" s="12" t="s">
         <v>403</v>
@@ -3408,7 +3408,7 @@
       <c r="B6" t="s">
         <v>302</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="36" t="s">
         <v>303</v>
       </c>
       <c r="D6" s="11" t="s">
@@ -3427,7 +3427,7 @@
         <v>6</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J6" s="12" t="s">
         <v>403</v>
@@ -3449,7 +3449,7 @@
       <c r="B7" t="s">
         <v>304</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="36" t="s">
         <v>305</v>
       </c>
       <c r="D7" s="11" t="s">
@@ -3468,7 +3468,7 @@
         <v>6</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J7" s="12" t="s">
         <v>403</v>
@@ -3490,7 +3490,7 @@
       <c r="B8" t="s">
         <v>306</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="36" t="s">
         <v>307</v>
       </c>
       <c r="D8" s="11" t="s">
@@ -3509,7 +3509,7 @@
         <v>6</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>403</v>
@@ -3531,7 +3531,7 @@
       <c r="B9" t="s">
         <v>308</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="36" t="s">
         <v>309</v>
       </c>
       <c r="D9" s="11" t="s">
@@ -3550,7 +3550,7 @@
         <v>6</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>403</v>
@@ -3572,7 +3572,7 @@
       <c r="B10" t="s">
         <v>310</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="36" t="s">
         <v>311</v>
       </c>
       <c r="D10" s="11" t="s">
@@ -3591,7 +3591,7 @@
         <v>6</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J10" s="12" t="s">
         <v>403</v>
@@ -3613,7 +3613,7 @@
       <c r="B11" t="s">
         <v>312</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="36" t="s">
         <v>313</v>
       </c>
       <c r="D11" s="11" t="s">
@@ -3632,7 +3632,7 @@
         <v>6</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>403</v>
@@ -3654,7 +3654,7 @@
       <c r="B12" t="s">
         <v>314</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="36" t="s">
         <v>315</v>
       </c>
       <c r="D12" s="11" t="s">
@@ -3673,7 +3673,7 @@
         <v>6</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>403</v>
@@ -3695,7 +3695,7 @@
       <c r="B13" t="s">
         <v>316</v>
       </c>
-      <c r="C13" s="46" t="s">
+      <c r="C13" s="36" t="s">
         <v>317</v>
       </c>
       <c r="D13" s="11" t="s">
@@ -3714,7 +3714,7 @@
         <v>6</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J13" s="12" t="s">
         <v>403</v>
@@ -3736,7 +3736,7 @@
       <c r="B14" t="s">
         <v>318</v>
       </c>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="36" t="s">
         <v>319</v>
       </c>
       <c r="D14" s="11" t="s">
@@ -3755,7 +3755,7 @@
         <v>6</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J14" s="12" t="s">
         <v>403</v>
@@ -3777,7 +3777,7 @@
       <c r="B15" t="s">
         <v>320</v>
       </c>
-      <c r="C15" s="46" t="s">
+      <c r="C15" s="36" t="s">
         <v>321</v>
       </c>
       <c r="D15" s="11" t="s">
@@ -3796,7 +3796,7 @@
         <v>6</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J15" s="12" t="s">
         <v>403</v>
@@ -3818,7 +3818,7 @@
       <c r="B16" t="s">
         <v>322</v>
       </c>
-      <c r="C16" s="46" t="s">
+      <c r="C16" s="36" t="s">
         <v>323</v>
       </c>
       <c r="D16" s="11" t="s">
@@ -3837,7 +3837,7 @@
         <v>6</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J16" s="12" t="s">
         <v>403</v>
@@ -3859,7 +3859,7 @@
       <c r="B17" t="s">
         <v>324</v>
       </c>
-      <c r="C17" s="46" t="s">
+      <c r="C17" s="36" t="s">
         <v>325</v>
       </c>
       <c r="D17" s="11" t="s">
@@ -3878,7 +3878,7 @@
         <v>6</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J17" s="12" t="s">
         <v>403</v>
@@ -3900,7 +3900,7 @@
       <c r="B18" t="s">
         <v>326</v>
       </c>
-      <c r="C18" s="46" t="s">
+      <c r="C18" s="36" t="s">
         <v>327</v>
       </c>
       <c r="D18" s="11" t="s">
@@ -3919,7 +3919,7 @@
         <v>6</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J18" s="12" t="s">
         <v>403</v>
@@ -3941,7 +3941,7 @@
       <c r="B19" t="s">
         <v>328</v>
       </c>
-      <c r="C19" s="46" t="s">
+      <c r="C19" s="36" t="s">
         <v>329</v>
       </c>
       <c r="D19" s="11" t="s">
@@ -3960,7 +3960,7 @@
         <v>6</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J19" s="12" t="s">
         <v>403</v>
@@ -3982,7 +3982,7 @@
       <c r="B20" t="s">
         <v>330</v>
       </c>
-      <c r="C20" s="46" t="s">
+      <c r="C20" s="36" t="s">
         <v>331</v>
       </c>
       <c r="D20" s="11" t="s">
@@ -4001,7 +4001,7 @@
         <v>6</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J20" s="12" t="s">
         <v>403</v>
@@ -4023,7 +4023,7 @@
       <c r="B21" t="s">
         <v>332</v>
       </c>
-      <c r="C21" s="46" t="s">
+      <c r="C21" s="36" t="s">
         <v>333</v>
       </c>
       <c r="D21" s="11" t="s">
@@ -4042,7 +4042,7 @@
         <v>6</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J21" s="12" t="s">
         <v>403</v>
@@ -4051,10 +4051,10 @@
         <v>404</v>
       </c>
       <c r="L21" s="12" t="s">
-        <v>443</v>
+        <v>511</v>
       </c>
       <c r="M21" s="12" t="s">
-        <v>444</v>
+        <v>509</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -4064,7 +4064,7 @@
       <c r="B22" t="s">
         <v>334</v>
       </c>
-      <c r="C22" s="46" t="s">
+      <c r="C22" s="36" t="s">
         <v>335</v>
       </c>
       <c r="D22" s="11" t="s">
@@ -4083,7 +4083,7 @@
         <v>6</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J22" s="12" t="s">
         <v>403</v>
@@ -4092,10 +4092,10 @@
         <v>404</v>
       </c>
       <c r="L22" s="12" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="M22" s="12" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -4105,7 +4105,7 @@
       <c r="B23" t="s">
         <v>336</v>
       </c>
-      <c r="C23" s="46" t="s">
+      <c r="C23" s="36" t="s">
         <v>337</v>
       </c>
       <c r="D23" s="11" t="s">
@@ -4124,7 +4124,7 @@
         <v>6</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J23" s="12" t="s">
         <v>403</v>
@@ -4133,10 +4133,10 @@
         <v>404</v>
       </c>
       <c r="L23" s="12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="M23" s="12" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
@@ -4146,7 +4146,7 @@
       <c r="B24" t="s">
         <v>338</v>
       </c>
-      <c r="C24" s="46" t="s">
+      <c r="C24" s="36" t="s">
         <v>339</v>
       </c>
       <c r="D24" s="11" t="s">
@@ -4165,7 +4165,7 @@
         <v>6</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J24" s="12" t="s">
         <v>403</v>
@@ -4174,10 +4174,10 @@
         <v>404</v>
       </c>
       <c r="L24" s="12" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="M24" s="12" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -4187,7 +4187,7 @@
       <c r="B25" t="s">
         <v>340</v>
       </c>
-      <c r="C25" s="46" t="s">
+      <c r="C25" s="36" t="s">
         <v>341</v>
       </c>
       <c r="D25" s="11" t="s">
@@ -4206,7 +4206,7 @@
         <v>6</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J25" s="12" t="s">
         <v>403</v>
@@ -4215,10 +4215,10 @@
         <v>404</v>
       </c>
       <c r="L25" s="12" t="s">
-        <v>451</v>
+        <v>512</v>
       </c>
       <c r="M25" s="12" t="s">
-        <v>452</v>
+        <v>510</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -4228,7 +4228,7 @@
       <c r="B26" t="s">
         <v>342</v>
       </c>
-      <c r="C26" s="46" t="s">
+      <c r="C26" s="36" t="s">
         <v>343</v>
       </c>
       <c r="D26" s="11" t="s">
@@ -4247,7 +4247,7 @@
         <v>6</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J26" s="12" t="s">
         <v>403</v>
@@ -4256,10 +4256,10 @@
         <v>404</v>
       </c>
       <c r="L26" s="12" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="M26" s="12" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
@@ -4269,7 +4269,7 @@
       <c r="B27" t="s">
         <v>344</v>
       </c>
-      <c r="C27" s="46" t="s">
+      <c r="C27" s="36" t="s">
         <v>345</v>
       </c>
       <c r="D27" s="11" t="s">
@@ -4288,7 +4288,7 @@
         <v>6</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J27" s="12" t="s">
         <v>403</v>
@@ -4297,10 +4297,10 @@
         <v>404</v>
       </c>
       <c r="L27" s="12" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="M27" s="12" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -4310,7 +4310,7 @@
       <c r="B28" t="s">
         <v>346</v>
       </c>
-      <c r="C28" s="46" t="s">
+      <c r="C28" s="36" t="s">
         <v>347</v>
       </c>
       <c r="D28" s="11" t="s">
@@ -4329,7 +4329,7 @@
         <v>6</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J28" s="12" t="s">
         <v>403</v>
@@ -4338,10 +4338,10 @@
         <v>404</v>
       </c>
       <c r="L28" s="12" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="M28" s="12" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
@@ -4351,7 +4351,7 @@
       <c r="B29" t="s">
         <v>348</v>
       </c>
-      <c r="C29" s="46" t="s">
+      <c r="C29" s="36" t="s">
         <v>349</v>
       </c>
       <c r="D29" s="11" t="s">
@@ -4370,7 +4370,7 @@
         <v>6</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J29" s="12" t="s">
         <v>403</v>
@@ -4379,10 +4379,10 @@
         <v>404</v>
       </c>
       <c r="L29" s="12" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="M29" s="12" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
@@ -4392,7 +4392,7 @@
       <c r="B30" t="s">
         <v>350</v>
       </c>
-      <c r="C30" s="46" t="s">
+      <c r="C30" s="36" t="s">
         <v>351</v>
       </c>
       <c r="D30" s="11" t="s">
@@ -4411,7 +4411,7 @@
         <v>6</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J30" s="12" t="s">
         <v>403</v>
@@ -4420,10 +4420,10 @@
         <v>404</v>
       </c>
       <c r="L30" s="12" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="M30" s="12" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -4433,7 +4433,7 @@
       <c r="B31" t="s">
         <v>352</v>
       </c>
-      <c r="C31" s="46" t="s">
+      <c r="C31" s="36" t="s">
         <v>353</v>
       </c>
       <c r="D31" s="11" t="s">
@@ -4452,7 +4452,7 @@
         <v>6</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J31" s="12" t="s">
         <v>403</v>
@@ -4461,10 +4461,10 @@
         <v>404</v>
       </c>
       <c r="L31" s="12" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="M31" s="12" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
@@ -4474,7 +4474,7 @@
       <c r="B32" t="s">
         <v>354</v>
       </c>
-      <c r="C32" s="46" t="s">
+      <c r="C32" s="36" t="s">
         <v>355</v>
       </c>
       <c r="D32" s="11" t="s">
@@ -4493,7 +4493,7 @@
         <v>6</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J32" s="12" t="s">
         <v>403</v>
@@ -4502,10 +4502,10 @@
         <v>404</v>
       </c>
       <c r="L32" s="12" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="M32" s="12" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
@@ -4515,7 +4515,7 @@
       <c r="B33" t="s">
         <v>356</v>
       </c>
-      <c r="C33" s="46" t="s">
+      <c r="C33" s="36" t="s">
         <v>357</v>
       </c>
       <c r="D33" s="11" t="s">
@@ -4534,7 +4534,7 @@
         <v>6</v>
       </c>
       <c r="I33" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J33" s="12" t="s">
         <v>403</v>
@@ -4543,10 +4543,10 @@
         <v>404</v>
       </c>
       <c r="L33" s="12" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="M33" s="12" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -4556,7 +4556,7 @@
       <c r="B34" t="s">
         <v>358</v>
       </c>
-      <c r="C34" s="46" t="s">
+      <c r="C34" s="36" t="s">
         <v>359</v>
       </c>
       <c r="D34" s="11" t="s">
@@ -4575,7 +4575,7 @@
         <v>6</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J34" s="12" t="s">
         <v>403</v>
@@ -4584,10 +4584,10 @@
         <v>404</v>
       </c>
       <c r="L34" s="12" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="M34" s="12" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
@@ -4597,7 +4597,7 @@
       <c r="B35" t="s">
         <v>360</v>
       </c>
-      <c r="C35" s="46" t="s">
+      <c r="C35" s="36" t="s">
         <v>361</v>
       </c>
       <c r="D35" s="11" t="s">
@@ -4616,7 +4616,7 @@
         <v>6</v>
       </c>
       <c r="I35" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J35" s="12" t="s">
         <v>403</v>
@@ -4625,10 +4625,10 @@
         <v>404</v>
       </c>
       <c r="L35" s="12" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="M35" s="12" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
@@ -4638,7 +4638,7 @@
       <c r="B36" t="s">
         <v>362</v>
       </c>
-      <c r="C36" s="46" t="s">
+      <c r="C36" s="36" t="s">
         <v>363</v>
       </c>
       <c r="D36" s="11" t="s">
@@ -4657,7 +4657,7 @@
         <v>6</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J36" s="12" t="s">
         <v>403</v>
@@ -4666,10 +4666,10 @@
         <v>404</v>
       </c>
       <c r="L36" s="12" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="M36" s="12" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
@@ -4679,7 +4679,7 @@
       <c r="B37" t="s">
         <v>364</v>
       </c>
-      <c r="C37" s="46" t="s">
+      <c r="C37" s="36" t="s">
         <v>365</v>
       </c>
       <c r="D37" s="11" t="s">
@@ -4698,7 +4698,7 @@
         <v>6</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J37" s="12" t="s">
         <v>403</v>
@@ -4707,10 +4707,10 @@
         <v>404</v>
       </c>
       <c r="L37" s="12" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="M37" s="12" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
@@ -4720,7 +4720,7 @@
       <c r="B38" t="s">
         <v>366</v>
       </c>
-      <c r="C38" s="46" t="s">
+      <c r="C38" s="36" t="s">
         <v>367</v>
       </c>
       <c r="D38" s="11" t="s">
@@ -4739,7 +4739,7 @@
         <v>6</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J38" s="12" t="s">
         <v>403</v>
@@ -4748,10 +4748,10 @@
         <v>404</v>
       </c>
       <c r="L38" s="12" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="M38" s="12" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
@@ -4761,7 +4761,7 @@
       <c r="B39" t="s">
         <v>368</v>
       </c>
-      <c r="C39" s="46" t="s">
+      <c r="C39" s="36" t="s">
         <v>369</v>
       </c>
       <c r="D39" s="11" t="s">
@@ -4780,7 +4780,7 @@
         <v>6</v>
       </c>
       <c r="I39" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J39" s="12" t="s">
         <v>403</v>
@@ -4789,10 +4789,10 @@
         <v>404</v>
       </c>
       <c r="L39" s="12" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="M39" s="12" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
@@ -4802,7 +4802,7 @@
       <c r="B40" t="s">
         <v>370</v>
       </c>
-      <c r="C40" s="46" t="s">
+      <c r="C40" s="36" t="s">
         <v>371</v>
       </c>
       <c r="D40" s="11" t="s">
@@ -4821,7 +4821,7 @@
         <v>6</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J40" s="12" t="s">
         <v>403</v>
@@ -4830,10 +4830,10 @@
         <v>404</v>
       </c>
       <c r="L40" s="12" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="M40" s="12" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
@@ -4843,7 +4843,7 @@
       <c r="B41" t="s">
         <v>372</v>
       </c>
-      <c r="C41" s="46" t="s">
+      <c r="C41" s="36" t="s">
         <v>373</v>
       </c>
       <c r="D41" s="11" t="s">
@@ -4862,7 +4862,7 @@
         <v>6</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J41" s="12" t="s">
         <v>403</v>
@@ -4871,10 +4871,10 @@
         <v>404</v>
       </c>
       <c r="L41" s="12" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="M41" s="12" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
@@ -4884,7 +4884,7 @@
       <c r="B42" t="s">
         <v>374</v>
       </c>
-      <c r="C42" s="46" t="s">
+      <c r="C42" s="36" t="s">
         <v>375</v>
       </c>
       <c r="D42" s="11" t="s">
@@ -4903,7 +4903,7 @@
         <v>6</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J42" s="12" t="s">
         <v>403</v>
@@ -4912,10 +4912,10 @@
         <v>404</v>
       </c>
       <c r="L42" s="12" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="M42" s="12" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
@@ -4925,7 +4925,7 @@
       <c r="B43" t="s">
         <v>376</v>
       </c>
-      <c r="C43" s="46" t="s">
+      <c r="C43" s="36" t="s">
         <v>377</v>
       </c>
       <c r="D43" s="11" t="s">
@@ -4944,7 +4944,7 @@
         <v>6</v>
       </c>
       <c r="I43" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J43" s="12" t="s">
         <v>403</v>
@@ -4953,10 +4953,10 @@
         <v>404</v>
       </c>
       <c r="L43" s="12" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="M43" s="12" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
@@ -4966,7 +4966,7 @@
       <c r="B44" t="s">
         <v>378</v>
       </c>
-      <c r="C44" s="46" t="s">
+      <c r="C44" s="36" t="s">
         <v>379</v>
       </c>
       <c r="D44" s="11" t="s">
@@ -4985,7 +4985,7 @@
         <v>6</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J44" s="12" t="s">
         <v>403</v>
@@ -4994,10 +4994,10 @@
         <v>404</v>
       </c>
       <c r="L44" s="12" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="M44" s="12" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
@@ -5007,7 +5007,7 @@
       <c r="B45" t="s">
         <v>380</v>
       </c>
-      <c r="C45" s="46" t="s">
+      <c r="C45" s="36" t="s">
         <v>381</v>
       </c>
       <c r="D45" s="11" t="s">
@@ -5026,7 +5026,7 @@
         <v>6</v>
       </c>
       <c r="I45" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J45" s="12" t="s">
         <v>403</v>
@@ -5035,10 +5035,10 @@
         <v>404</v>
       </c>
       <c r="L45" s="12" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="M45" s="12" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
@@ -5048,7 +5048,7 @@
       <c r="B46" t="s">
         <v>382</v>
       </c>
-      <c r="C46" s="46" t="s">
+      <c r="C46" s="36" t="s">
         <v>383</v>
       </c>
       <c r="D46" s="11" t="s">
@@ -5067,7 +5067,7 @@
         <v>6</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J46" s="12" t="s">
         <v>403</v>
@@ -5076,10 +5076,10 @@
         <v>404</v>
       </c>
       <c r="L46" s="12" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="M46" s="12" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
@@ -5089,7 +5089,7 @@
       <c r="B47" t="s">
         <v>384</v>
       </c>
-      <c r="C47" s="46" t="s">
+      <c r="C47" s="36" t="s">
         <v>385</v>
       </c>
       <c r="D47" s="11" t="s">
@@ -5108,7 +5108,7 @@
         <v>6</v>
       </c>
       <c r="I47" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J47" s="12" t="s">
         <v>403</v>
@@ -5117,10 +5117,10 @@
         <v>404</v>
       </c>
       <c r="L47" s="12" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="M47" s="12" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
@@ -5130,7 +5130,7 @@
       <c r="B48" t="s">
         <v>386</v>
       </c>
-      <c r="C48" s="46" t="s">
+      <c r="C48" s="36" t="s">
         <v>387</v>
       </c>
       <c r="D48" s="11" t="s">
@@ -5149,7 +5149,7 @@
         <v>6</v>
       </c>
       <c r="I48" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J48" s="12" t="s">
         <v>403</v>
@@ -5158,10 +5158,10 @@
         <v>404</v>
       </c>
       <c r="L48" s="12" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="M48" s="12" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
@@ -5171,7 +5171,7 @@
       <c r="B49" t="s">
         <v>388</v>
       </c>
-      <c r="C49" s="46" t="s">
+      <c r="C49" s="36" t="s">
         <v>389</v>
       </c>
       <c r="D49" s="11" t="s">
@@ -5190,7 +5190,7 @@
         <v>6</v>
       </c>
       <c r="I49" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J49" s="12" t="s">
         <v>403</v>
@@ -5199,10 +5199,10 @@
         <v>404</v>
       </c>
       <c r="L49" s="12" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="M49" s="12" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
@@ -5212,7 +5212,7 @@
       <c r="B50" t="s">
         <v>390</v>
       </c>
-      <c r="C50" s="46" t="s">
+      <c r="C50" s="36" t="s">
         <v>391</v>
       </c>
       <c r="D50" s="11" t="s">
@@ -5231,7 +5231,7 @@
         <v>6</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J50" s="12" t="s">
         <v>403</v>
@@ -5240,10 +5240,10 @@
         <v>404</v>
       </c>
       <c r="L50" s="12" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="M50" s="12" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
@@ -5253,7 +5253,7 @@
       <c r="B51" t="s">
         <v>392</v>
       </c>
-      <c r="C51" s="46" t="s">
+      <c r="C51" s="36" t="s">
         <v>393</v>
       </c>
       <c r="D51" s="11" t="s">
@@ -5272,7 +5272,7 @@
         <v>6</v>
       </c>
       <c r="I51" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J51" s="12" t="s">
         <v>403</v>
@@ -5281,10 +5281,10 @@
         <v>404</v>
       </c>
       <c r="L51" s="12" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="M51" s="12" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
@@ -5294,7 +5294,7 @@
       <c r="B52" t="s">
         <v>394</v>
       </c>
-      <c r="C52" s="46" t="s">
+      <c r="C52" s="36" t="s">
         <v>395</v>
       </c>
       <c r="D52" s="11" t="s">
@@ -5313,7 +5313,7 @@
         <v>6</v>
       </c>
       <c r="I52" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J52" s="12" t="s">
         <v>403</v>
@@ -5322,10 +5322,10 @@
         <v>404</v>
       </c>
       <c r="L52" s="12" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="M52" s="12" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
@@ -5335,7 +5335,7 @@
       <c r="B53" t="s">
         <v>396</v>
       </c>
-      <c r="C53" s="46" t="s">
+      <c r="C53" s="36" t="s">
         <v>397</v>
       </c>
       <c r="D53" s="11" t="s">
@@ -5354,7 +5354,7 @@
         <v>6</v>
       </c>
       <c r="I53" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J53" s="12" t="s">
         <v>403</v>
@@ -5363,10 +5363,10 @@
         <v>404</v>
       </c>
       <c r="L53" s="12" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="M53" s="12" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
@@ -5376,7 +5376,7 @@
       <c r="B54" t="s">
         <v>398</v>
       </c>
-      <c r="C54" s="46" t="s">
+      <c r="C54" s="36" t="s">
         <v>399</v>
       </c>
       <c r="D54" s="11" t="s">
@@ -5395,7 +5395,7 @@
         <v>6</v>
       </c>
       <c r="I54" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J54" s="12" t="s">
         <v>403</v>
@@ -5404,10 +5404,10 @@
         <v>404</v>
       </c>
       <c r="L54" s="12" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="M54" s="12" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
@@ -5417,7 +5417,7 @@
       <c r="B55" t="s">
         <v>400</v>
       </c>
-      <c r="C55" s="46" t="s">
+      <c r="C55" s="36" t="s">
         <v>401</v>
       </c>
       <c r="D55" s="11" t="s">
@@ -5436,7 +5436,7 @@
         <v>6</v>
       </c>
       <c r="I55" s="11" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="J55" s="12" t="s">
         <v>403</v>
@@ -5445,10 +5445,10 @@
         <v>404</v>
       </c>
       <c r="L55" s="12" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="M55" s="12" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
@@ -7602,15 +7602,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
     </row>
     <row r="2" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="43"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="44"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -7622,172 +7622,172 @@
       <c r="A3" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="41"/>
+      <c r="C3" s="42"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="41"/>
+      <c r="C4" s="42"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="41"/>
+      <c r="C5" s="42"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="C6" s="41"/>
+      <c r="C6" s="42"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="41"/>
+      <c r="C7" s="42"/>
     </row>
     <row r="8" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="41"/>
+      <c r="C8" s="42"/>
     </row>
     <row r="9" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="41"/>
+      <c r="C9" s="42"/>
     </row>
     <row r="10" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="C10" s="41"/>
+      <c r="C10" s="42"/>
     </row>
     <row r="11" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="41"/>
+      <c r="C11" s="42"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="C12" s="41"/>
+      <c r="C12" s="42"/>
     </row>
     <row r="13" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="41"/>
+      <c r="C13" s="42"/>
     </row>
     <row r="14" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="41"/>
+      <c r="C14" s="42"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="41"/>
+      <c r="C15" s="42"/>
     </row>
     <row r="16" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="C16" s="41"/>
+      <c r="C16" s="42"/>
     </row>
     <row r="17" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="C17" s="41"/>
+      <c r="C17" s="42"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="C18" s="41"/>
+      <c r="C18" s="42"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="C19" s="41"/>
+      <c r="C19" s="42"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="41" t="s">
+      <c r="B20" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="C20" s="41"/>
+      <c r="C20" s="42"/>
     </row>
     <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A21" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="42" t="s">
         <v>128</v>
       </c>
-      <c r="C21" s="41"/>
+      <c r="C21" s="42"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -7799,28 +7799,28 @@
       <c r="A22" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="42" t="s">
         <v>129</v>
       </c>
-      <c r="C22" s="41"/>
+      <c r="C22" s="42"/>
     </row>
     <row r="23" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="C23" s="41"/>
+      <c r="C23" s="42"/>
     </row>
     <row r="24" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="42" t="s">
         <v>131</v>
       </c>
-      <c r="C24" s="41"/>
+      <c r="C24" s="42"/>
     </row>
     <row r="25" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
@@ -7924,10 +7924,10 @@
       <c r="A37" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B37" s="44" t="s">
+      <c r="B37" s="45" t="s">
         <v>284</v>
       </c>
-      <c r="C37" s="44"/>
+      <c r="C37" s="45"/>
       <c r="D37" s="34"/>
       <c r="E37" s="34"/>
       <c r="F37" s="34"/>
@@ -7972,11 +7972,11 @@
       <c r="A42" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="B42" s="44" t="s">
+      <c r="B42" s="45" t="s">
         <v>290</v>
       </c>
-      <c r="C42" s="44"/>
-      <c r="D42" s="44"/>
+      <c r="C42" s="45"/>
+      <c r="D42" s="45"/>
       <c r="E42" s="34"/>
       <c r="F42" s="34"/>
       <c r="G42" s="34"/>
@@ -7987,75 +7987,75 @@
       <c r="A43" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="B43" s="41" t="s">
+      <c r="B43" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="C43" s="41"/>
+      <c r="C43" s="42"/>
     </row>
     <row r="44" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="41"/>
-      <c r="C44" s="41"/>
+      <c r="B44" s="42"/>
+      <c r="C44" s="42"/>
     </row>
     <row r="45" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A45" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="42"/>
-      <c r="C45" s="43"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="44"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="B46" s="41" t="s">
+      <c r="B46" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="C46" s="41"/>
+      <c r="C46" s="42"/>
     </row>
     <row r="47" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="B47" s="41" t="s">
+      <c r="B47" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="C47" s="41"/>
+      <c r="C47" s="42"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A48" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="41" t="s">
+      <c r="B48" s="42" t="s">
         <v>135</v>
       </c>
-      <c r="C48" s="41"/>
+      <c r="C48" s="42"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="B49" s="41" t="s">
+      <c r="B49" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="C49" s="41"/>
+      <c r="C49" s="42"/>
     </row>
     <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="41" t="s">
+      <c r="B50" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="C50" s="41"/>
+      <c r="C50" s="42"/>
     </row>
     <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="B51" s="41" t="s">
+      <c r="B51" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="C51" s="41"/>
+      <c r="C51" s="42"/>
     </row>
     <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
@@ -8071,264 +8071,264 @@
       <c r="A54" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="B54" s="41" t="s">
+      <c r="B54" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="C54" s="41"/>
+      <c r="C54" s="42"/>
     </row>
     <row r="55" spans="1:3" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="41"/>
-      <c r="C55" s="41"/>
+      <c r="B55" s="42"/>
+      <c r="C55" s="42"/>
     </row>
     <row r="56" spans="1:3" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A56" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B56" s="45"/>
-      <c r="C56" s="41"/>
+      <c r="B56" s="46"/>
+      <c r="C56" s="42"/>
     </row>
     <row r="57" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="B57" s="41" t="s">
+      <c r="B57" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="C57" s="41"/>
+      <c r="C57" s="42"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A58" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B58" s="41" t="s">
+      <c r="B58" s="42" t="s">
         <v>141</v>
       </c>
-      <c r="C58" s="41"/>
+      <c r="C58" s="42"/>
     </row>
     <row r="59" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="B59" s="41" t="s">
+      <c r="B59" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="C59" s="41"/>
+      <c r="C59" s="42"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A60" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="B60" s="41" t="s">
+      <c r="B60" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="C60" s="41"/>
+      <c r="C60" s="42"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A61" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="B61" s="41" t="s">
+      <c r="B61" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="C61" s="41"/>
+      <c r="C61" s="42"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A62" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="B62" s="41" t="s">
+      <c r="B62" s="42" t="s">
         <v>145</v>
       </c>
-      <c r="C62" s="41"/>
+      <c r="C62" s="42"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A63" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="B63" s="41" t="s">
+      <c r="B63" s="42" t="s">
         <v>146</v>
       </c>
-      <c r="C63" s="41"/>
+      <c r="C63" s="42"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A64" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="B64" s="41" t="s">
+      <c r="B64" s="42" t="s">
         <v>147</v>
       </c>
-      <c r="C64" s="41"/>
+      <c r="C64" s="42"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A65" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="B65" s="41" t="s">
+      <c r="B65" s="42" t="s">
         <v>148</v>
       </c>
-      <c r="C65" s="41"/>
+      <c r="C65" s="42"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A66" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="B66" s="41" t="s">
+      <c r="B66" s="42" t="s">
         <v>149</v>
       </c>
-      <c r="C66" s="41"/>
+      <c r="C66" s="42"/>
     </row>
     <row r="67" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B67" s="41" t="s">
+      <c r="B67" s="42" t="s">
         <v>150</v>
       </c>
-      <c r="C67" s="41"/>
+      <c r="C67" s="42"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A68" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B68" s="41" t="s">
+      <c r="B68" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="C68" s="41"/>
+      <c r="C68" s="42"/>
     </row>
     <row r="69" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="B69" s="41" t="s">
+      <c r="B69" s="42" t="s">
         <v>152</v>
       </c>
-      <c r="C69" s="41"/>
+      <c r="C69" s="42"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A70" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="B70" s="41" t="s">
+      <c r="B70" s="42" t="s">
         <v>153</v>
       </c>
-      <c r="C70" s="41"/>
+      <c r="C70" s="42"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A71" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="B71" s="41" t="s">
+      <c r="B71" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="C71" s="41"/>
+      <c r="C71" s="42"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A72" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="B72" s="41" t="s">
+      <c r="B72" s="42" t="s">
         <v>155</v>
       </c>
-      <c r="C72" s="41"/>
+      <c r="C72" s="42"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A73" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="B73" s="41" t="s">
+      <c r="B73" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="C73" s="41"/>
+      <c r="C73" s="42"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A74" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="B74" s="41" t="s">
+      <c r="B74" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="C74" s="41"/>
+      <c r="C74" s="42"/>
     </row>
     <row r="75" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="B75" s="41" t="s">
+      <c r="B75" s="42" t="s">
         <v>158</v>
       </c>
-      <c r="C75" s="41"/>
+      <c r="C75" s="42"/>
     </row>
     <row r="76" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="B76" s="41" t="s">
+      <c r="B76" s="42" t="s">
         <v>159</v>
       </c>
-      <c r="C76" s="41"/>
+      <c r="C76" s="42"/>
     </row>
     <row r="77" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="B77" s="41" t="s">
+      <c r="B77" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="C77" s="41"/>
+      <c r="C77" s="42"/>
     </row>
     <row r="78" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="B78" s="41" t="s">
+      <c r="B78" s="42" t="s">
         <v>161</v>
       </c>
-      <c r="C78" s="41"/>
+      <c r="C78" s="42"/>
     </row>
     <row r="79" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="B79" s="41" t="s">
+      <c r="B79" s="42" t="s">
         <v>162</v>
       </c>
-      <c r="C79" s="41"/>
+      <c r="C79" s="42"/>
     </row>
     <row r="80" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="B80" s="41" t="s">
+      <c r="B80" s="42" t="s">
         <v>163</v>
       </c>
-      <c r="C80" s="41"/>
+      <c r="C80" s="42"/>
     </row>
     <row r="81" spans="1:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="B81" s="41" t="s">
+      <c r="B81" s="42" t="s">
         <v>164</v>
       </c>
-      <c r="C81" s="41"/>
+      <c r="C81" s="42"/>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A82" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B82" s="41" t="s">
+      <c r="B82" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="C82" s="41"/>
+      <c r="C82" s="42"/>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A83" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B83" s="41" t="s">
+      <c r="B83" s="42" t="s">
         <v>166</v>
       </c>
-      <c r="C83" s="41"/>
+      <c r="C83" s="42"/>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A84" s="2" t="s">

</xml_diff>